<commit_message>
Añadido MostPop cold_start y emisiones
</commit_message>
<xml_diff>
--- a/baselines_results.xlsx
+++ b/baselines_results.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DE2FC3-B135-4C21-9DC0-712691230904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
   <si>
-    <t>M.Pop</t>
-  </si>
-  <si>
     <t>BiVAECF</t>
   </si>
   <si>
@@ -86,13 +89,16 @@
   </si>
   <si>
     <t>NDCG@10</t>
+  </si>
+  <si>
+    <t>MostPop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,8 +150,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -155,13 +164,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -199,7 +216,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -233,6 +250,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -267,9 +285,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -442,811 +461,813 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>2.1669415429723199E-2</v>
+      </c>
+      <c r="E2">
+        <v>2.51969946857247E-2</v>
+      </c>
+      <c r="F2">
+        <v>0.15408911228042621</v>
+      </c>
+      <c r="G2">
+        <v>0.50627517700195313</v>
+      </c>
+      <c r="H2">
+        <v>0.56358039379119873</v>
+      </c>
+      <c r="I2">
+        <v>2.10750643163919E-2</v>
+      </c>
+      <c r="J2">
+        <v>2.1430263295769601E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2">
-        <v>0.0216694154297232</v>
-      </c>
-      <c r="E2">
-        <v>0.0251969946857247</v>
-      </c>
-      <c r="F2">
-        <v>0.1540891122804262</v>
-      </c>
-      <c r="G2">
-        <v>0.5062751770019531</v>
-      </c>
-      <c r="H2">
-        <v>0.5635803937911987</v>
-      </c>
-      <c r="I2">
-        <v>0.0210750643163919</v>
-      </c>
-      <c r="J2">
-        <v>0.0214302632957696</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D3">
-        <v>0.0369525380245556</v>
+        <v>3.6952538024555601E-2</v>
       </c>
       <c r="E3">
-        <v>0.0427661718893164</v>
+        <v>4.2766171889316397E-2</v>
       </c>
       <c r="F3">
-        <v>0.1991135239142386</v>
+        <v>0.19911352391423859</v>
       </c>
       <c r="G3">
-        <v>0.5653563737869263</v>
+        <v>0.56535637378692627</v>
       </c>
       <c r="H3">
         <v>0.6230168342590332</v>
       </c>
       <c r="I3">
-        <v>0.0497276820242404</v>
+        <v>4.9727682024240397E-2</v>
       </c>
       <c r="J3">
-        <v>0.0493724830448627</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+        <v>4.9372483044862699E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4">
-        <v>0.0170872724459561</v>
+        <v>1.7087272445956099E-2</v>
       </c>
       <c r="E4">
-        <v>0.0191770842858194</v>
+        <v>1.91770842858194E-2</v>
       </c>
       <c r="F4">
         <v>0.1371091224867218</v>
       </c>
       <c r="G4">
-        <v>0.4489425420761108</v>
+        <v>0.44894254207611078</v>
       </c>
       <c r="H4">
-        <v>0.5097736716270447</v>
+        <v>0.50977367162704468</v>
       </c>
       <c r="I4">
-        <v>0.020696472376585</v>
+        <v>2.0696472376585E-2</v>
       </c>
       <c r="J4">
-        <v>0.0204380638897418</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>2.04380638897418E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>0.1939317319848293</v>
       </c>
       <c r="E5">
-        <v>0.09747155499367879</v>
+        <v>9.7471554993678794E-2</v>
       </c>
       <c r="F5">
-        <v>0.7097345132743362</v>
+        <v>0.70973451327433623</v>
       </c>
       <c r="G5">
-        <v>0.6228955984115601</v>
+        <v>0.62289559841156006</v>
       </c>
       <c r="H5">
-        <v>0.7070707082748413</v>
+        <v>0.70707070827484131</v>
       </c>
       <c r="I5">
-        <v>0.189450055360794</v>
+        <v>0.18945005536079401</v>
       </c>
       <c r="J5">
-        <v>0.1901234537363052</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+        <v>0.19012345373630521</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6">
-        <v>0.2638432364096081</v>
+        <v>0.26384323640960811</v>
       </c>
       <c r="E6">
-        <v>0.278204804045512</v>
+        <v>0.27820480404551201</v>
       </c>
       <c r="F6">
-        <v>0.7187104930467763</v>
+        <v>0.71871049304677626</v>
       </c>
       <c r="G6">
-        <v>0.7135802507400513</v>
+        <v>0.71358025074005127</v>
       </c>
       <c r="H6">
         <v>0.7905724048614502</v>
       </c>
       <c r="I6">
-        <v>0.3012345731258392</v>
+        <v>0.30123457312583918</v>
       </c>
       <c r="J6">
-        <v>0.3326599299907684</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+        <v>0.33265992999076838</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7">
-        <v>0.2015540551425598</v>
+        <v>0.20155405514255981</v>
       </c>
       <c r="E7">
         <v>0.1205563599001164</v>
       </c>
       <c r="F7">
-        <v>0.7025763870124153</v>
+        <v>0.70257638701241532</v>
       </c>
       <c r="G7">
         <v>0.4836084246635437</v>
       </c>
       <c r="H7">
-        <v>0.5582916140556335</v>
+        <v>0.55829161405563354</v>
       </c>
       <c r="I7">
-        <v>0.1793625354766845</v>
+        <v>0.17936253547668449</v>
       </c>
       <c r="J7">
-        <v>0.1903207749128341</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>0.19032077491283411</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8">
-        <v>0.5570253646583552</v>
+        <v>0.55702536465835517</v>
       </c>
       <c r="E8">
-        <v>0.5461151792957782</v>
+        <v>0.54611517929577824</v>
       </c>
       <c r="F8">
-        <v>0.5814597214239596</v>
+        <v>0.58145972142395963</v>
       </c>
       <c r="G8">
-        <v>0.9117713570594788</v>
+        <v>0.91177135705947876</v>
       </c>
       <c r="H8">
         <v>0.9290555715560912</v>
       </c>
       <c r="I8">
-        <v>0.9288296699523926</v>
+        <v>0.92882966995239258</v>
       </c>
       <c r="J8">
-        <v>0.9151604175567628</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+        <v>0.91516041755676281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9">
-        <v>0.742965824883572</v>
+        <v>0.74296582488357199</v>
       </c>
       <c r="E9">
-        <v>0.7304254682551508</v>
+        <v>0.73042546825515076</v>
       </c>
       <c r="F9">
-        <v>0.7490459870433051</v>
+        <v>0.74904598704330505</v>
       </c>
       <c r="G9">
         <v>0.9489380717277528</v>
       </c>
       <c r="H9">
-        <v>0.96384996175766</v>
+        <v>0.96384996175766002</v>
       </c>
       <c r="I9">
-        <v>0.9596701264381408</v>
+        <v>0.95967012643814076</v>
       </c>
       <c r="J9">
-        <v>0.9497288465499878</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+        <v>0.94972884654998779</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10">
-        <v>0.4892838894006368</v>
+        <v>0.48928388940063677</v>
       </c>
       <c r="E10">
-        <v>0.4717008755416678</v>
+        <v>0.47170087554166779</v>
       </c>
       <c r="F10">
-        <v>0.4955748687738332</v>
+        <v>0.49557486877383322</v>
       </c>
       <c r="G10">
-        <v>0.830578088760376</v>
+        <v>0.83057808876037598</v>
       </c>
       <c r="H10">
         <v>0.8464432954788208</v>
       </c>
       <c r="I10">
-        <v>0.849577784538269</v>
+        <v>0.84957778453826904</v>
       </c>
       <c r="J10">
-        <v>0.8439829349517822</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>0.84398293495178223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11">
-        <v>0.4911513413920091</v>
+        <v>0.49115134139200911</v>
       </c>
       <c r="E11">
-        <v>0.4384763667720795</v>
+        <v>0.43847636677207952</v>
       </c>
       <c r="F11">
-        <v>0.5317925916499152</v>
+        <v>0.53179259164991521</v>
       </c>
       <c r="G11">
-        <v>0.9086970686912536</v>
+        <v>0.90869706869125355</v>
       </c>
       <c r="H11">
-        <v>0.9282327890396118</v>
+        <v>0.92823278903961182</v>
       </c>
       <c r="I11">
         <v>0.9258623719215392</v>
       </c>
       <c r="J11">
-        <v>0.9105770587921144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+        <v>0.91057705879211437</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12">
-        <v>0.6585527928264068</v>
+        <v>0.65855279282640677</v>
       </c>
       <c r="E12">
-        <v>0.6175784220217966</v>
+        <v>0.61757842202179658</v>
       </c>
       <c r="F12">
-        <v>0.6824305334140393</v>
+        <v>0.68243053341403925</v>
       </c>
       <c r="G12">
-        <v>0.9495667815208436</v>
+        <v>0.94956678152084362</v>
       </c>
       <c r="H12">
-        <v>0.9646885991096495</v>
+        <v>0.96468859910964955</v>
       </c>
       <c r="I12">
-        <v>0.9588033556938172</v>
+        <v>0.95880335569381725</v>
       </c>
       <c r="J12">
         <v>0.947196364402771</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13">
-        <v>0.4281502647287516</v>
+        <v>0.42815026472875162</v>
       </c>
       <c r="E13">
         <v>0.3871233884163604</v>
       </c>
       <c r="F13">
-        <v>0.4533504536994604</v>
+        <v>0.45335045369946042</v>
       </c>
       <c r="G13">
-        <v>0.8322452306747437</v>
+        <v>0.83224523067474365</v>
       </c>
       <c r="H13">
-        <v>0.8555105924606323</v>
+        <v>0.85551059246063232</v>
       </c>
       <c r="I13">
-        <v>0.858952522277832</v>
+        <v>0.85895252227783203</v>
       </c>
       <c r="J13">
-        <v>0.8516348004341125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>0.85163480043411255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>0.54754122874476652</v>
+      </c>
+      <c r="E14">
+        <v>0.53568056420209709</v>
+      </c>
+      <c r="F14">
+        <v>0.56091707254550127</v>
+      </c>
+      <c r="G14">
+        <v>0.92730093002319336</v>
+      </c>
+      <c r="H14">
+        <v>0.94983124732971203</v>
+      </c>
+      <c r="I14">
+        <v>0.95065218210220337</v>
+      </c>
+      <c r="J14">
+        <v>0.94919276237487804</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D14">
-        <v>0.5475412287447665</v>
-      </c>
-      <c r="E14">
-        <v>0.5356805642020971</v>
-      </c>
-      <c r="F14">
-        <v>0.5609170725455013</v>
-      </c>
-      <c r="G14">
-        <v>0.9273009300231934</v>
-      </c>
-      <c r="H14">
-        <v>0.949831247329712</v>
-      </c>
-      <c r="I14">
-        <v>0.9506521821022034</v>
-      </c>
-      <c r="J14">
-        <v>0.949192762374878</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1" t="s">
+      <c r="D15">
+        <v>0.73153815871388295</v>
+      </c>
+      <c r="E15">
+        <v>0.72606703409382212</v>
+      </c>
+      <c r="F15">
+        <v>0.74259347420075394</v>
+      </c>
+      <c r="G15">
+        <v>0.96323996782302856</v>
+      </c>
+      <c r="H15">
+        <v>0.97445952892303478</v>
+      </c>
+      <c r="I15">
+        <v>0.97418588399887085</v>
+      </c>
+      <c r="J15">
+        <v>0.97154062986373901</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D15">
-        <v>0.7315381587138829</v>
-      </c>
-      <c r="E15">
-        <v>0.7260670340938221</v>
-      </c>
-      <c r="F15">
-        <v>0.7425934742007539</v>
-      </c>
-      <c r="G15">
-        <v>0.9632399678230286</v>
-      </c>
-      <c r="H15">
-        <v>0.9744595289230348</v>
-      </c>
-      <c r="I15">
-        <v>0.9741858839988708</v>
-      </c>
-      <c r="J15">
-        <v>0.971540629863739</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D16">
         <v>0.4749401630470052</v>
       </c>
       <c r="E16">
-        <v>0.4639011187425697</v>
+        <v>0.46390111874256967</v>
       </c>
       <c r="F16">
-        <v>0.4915565742845703</v>
+        <v>0.49155657428457028</v>
       </c>
       <c r="G16">
-        <v>0.847109854221344</v>
+        <v>0.84710985422134399</v>
       </c>
       <c r="H16">
-        <v>0.8767202496528625</v>
+        <v>0.87672024965286255</v>
       </c>
       <c r="I16">
-        <v>0.8786603808403015</v>
+        <v>0.87866038084030151</v>
       </c>
       <c r="J16">
-        <v>0.8795891404151917</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
-        <v>18</v>
+        <v>0.87958914041519165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>0.68465476048600815</v>
+      </c>
+      <c r="E17">
+        <v>0.67889930254070396</v>
+      </c>
+      <c r="F17">
+        <v>0.70757458387955308</v>
+      </c>
+      <c r="G17">
+        <v>0.93834871053695679</v>
+      </c>
+      <c r="H17">
+        <v>0.95070612430572521</v>
+      </c>
+      <c r="I17">
+        <v>0.95233571529388439</v>
+      </c>
+      <c r="J17">
+        <v>0.95247149467468262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D17">
-        <v>0.6846547604860082</v>
-      </c>
-      <c r="E17">
-        <v>0.678899302540704</v>
-      </c>
-      <c r="F17">
-        <v>0.7075745838795531</v>
-      </c>
-      <c r="G17">
-        <v>0.9383487105369568</v>
-      </c>
-      <c r="H17">
-        <v>0.9507061243057252</v>
-      </c>
-      <c r="I17">
-        <v>0.9523357152938844</v>
-      </c>
-      <c r="J17">
-        <v>0.9524714946746826</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D18">
-        <v>0.8415243656752417</v>
+        <v>0.84152436567524169</v>
       </c>
       <c r="E18">
-        <v>0.8395558449813008</v>
+        <v>0.83955584498130076</v>
       </c>
       <c r="F18">
-        <v>0.8472114396944569</v>
+        <v>0.84721143969445689</v>
       </c>
       <c r="G18">
-        <v>0.9713470935821532</v>
+        <v>0.97134709358215321</v>
       </c>
       <c r="H18">
-        <v>0.9767789244651794</v>
+        <v>0.97677892446517944</v>
       </c>
       <c r="I18">
         <v>0.9762357473373412</v>
       </c>
       <c r="J18">
-        <v>0.9755567908287048</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+        <v>0.97555679082870483</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19">
         <v>0.6051443788294556</v>
       </c>
       <c r="E19">
-        <v>0.5977890993255521</v>
+        <v>0.59778909932555213</v>
       </c>
       <c r="F19">
-        <v>0.6168846272809396</v>
+        <v>0.61688462728093962</v>
       </c>
       <c r="G19">
-        <v>0.8666979074478149</v>
+        <v>0.86669790744781494</v>
       </c>
       <c r="H19">
-        <v>0.8845361471176147</v>
+        <v>0.88453614711761475</v>
       </c>
       <c r="I19">
-        <v>0.8914504051208496</v>
+        <v>0.89145040512084961</v>
       </c>
       <c r="J19">
-        <v>0.8933619260787964</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>0.89336192607879639</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20">
-        <v>0.5026983435500099</v>
+        <v>0.50269834355000986</v>
       </c>
       <c r="E20">
-        <v>0.4798940646468419</v>
+        <v>0.47989406464684192</v>
       </c>
       <c r="F20">
         <v>0.5316462851749284</v>
       </c>
       <c r="G20">
-        <v>0.9303986430168152</v>
+        <v>0.93039864301681519</v>
       </c>
       <c r="H20">
-        <v>0.9428571462631226</v>
+        <v>0.94285714626312256</v>
       </c>
       <c r="I20">
-        <v>0.9509966969490052</v>
+        <v>0.95099669694900524</v>
       </c>
       <c r="J20">
-        <v>0.9426910281181335</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+        <v>0.94269102811813354</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21">
+        <v>0.72091600889248431</v>
+      </c>
+      <c r="E21">
+        <v>0.71660114855497103</v>
+      </c>
+      <c r="F21">
+        <v>0.72716373996051586</v>
+      </c>
+      <c r="G21">
+        <v>0.96495014429092396</v>
+      </c>
+      <c r="H21">
+        <v>0.97790700197219838</v>
+      </c>
+      <c r="I21">
+        <v>0.97491693496704102</v>
+      </c>
+      <c r="J21">
+        <v>0.97059798240661621</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D21">
-        <v>0.7209160088924843</v>
-      </c>
-      <c r="E21">
-        <v>0.716601148554971</v>
-      </c>
-      <c r="F21">
-        <v>0.7271637399605159</v>
-      </c>
-      <c r="G21">
-        <v>0.964950144290924</v>
-      </c>
-      <c r="H21">
-        <v>0.9779070019721984</v>
-      </c>
-      <c r="I21">
-        <v>0.974916934967041</v>
-      </c>
-      <c r="J21">
-        <v>0.9705979824066162</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D22">
-        <v>0.4379165120935851</v>
+        <v>0.43791651209358512</v>
       </c>
       <c r="E22">
-        <v>0.4071620976319325</v>
+        <v>0.40716209763193251</v>
       </c>
       <c r="F22">
-        <v>0.4515171768950008</v>
+        <v>0.45151717689500082</v>
       </c>
       <c r="G22">
-        <v>0.8497676253318787</v>
+        <v>0.84976762533187866</v>
       </c>
       <c r="H22">
-        <v>0.8750119209289551</v>
+        <v>0.87501192092895508</v>
       </c>
       <c r="I22">
-        <v>0.8792068362236023</v>
+        <v>0.87920683622360229</v>
       </c>
       <c r="J22">
-        <v>0.8726711869239807</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="1" t="s">
+        <v>0.87267118692398071</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23">
+        <v>0.18946346896346891</v>
+      </c>
+      <c r="E23">
+        <v>0.18657994257994251</v>
+      </c>
+      <c r="F23">
+        <v>0.18197569547569539</v>
+      </c>
+      <c r="G23">
+        <v>0.61951619386672974</v>
+      </c>
+      <c r="H23">
+        <v>0.67773675918579102</v>
+      </c>
+      <c r="I23">
+        <v>0.65395653247833252</v>
+      </c>
+      <c r="J23">
+        <v>0.62648624181747437</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D23">
-        <v>0.1894634689634689</v>
-      </c>
-      <c r="E23">
-        <v>0.1865799425799425</v>
-      </c>
-      <c r="F23">
-        <v>0.1819756954756954</v>
-      </c>
-      <c r="G23">
-        <v>0.6195161938667297</v>
-      </c>
-      <c r="H23">
-        <v>0.677736759185791</v>
-      </c>
-      <c r="I23">
-        <v>0.6539565324783325</v>
-      </c>
-      <c r="J23">
-        <v>0.6264862418174744</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D24">
-        <v>0.2686013266013266</v>
+        <v>0.26860132660132657</v>
       </c>
       <c r="E24">
-        <v>0.2749020889020889</v>
+        <v>0.27490208890208889</v>
       </c>
       <c r="F24">
-        <v>0.269515741015741</v>
+        <v>0.26951574101574099</v>
       </c>
       <c r="G24">
-        <v>0.7187371850013733</v>
+        <v>0.71873718500137329</v>
       </c>
       <c r="H24">
-        <v>0.7716277241706848</v>
+        <v>0.77162772417068481</v>
       </c>
       <c r="I24">
         <v>0.7515375018119812</v>
       </c>
       <c r="J24">
-        <v>0.7105370759963989</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+        <v>0.71053707599639893</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25">
         <v>0.1654424235762732</v>
       </c>
       <c r="E25">
-        <v>0.169375458377363</v>
+        <v>0.16937545837736301</v>
       </c>
       <c r="F25">
-        <v>0.165435473489649</v>
+        <v>0.16543547348964899</v>
       </c>
       <c r="G25">
-        <v>0.537446916103363</v>
+        <v>0.53744691610336304</v>
       </c>
       <c r="H25">
-        <v>0.5920780301094055</v>
+        <v>0.59207803010940552</v>
       </c>
       <c r="I25">
-        <v>0.5769718885421753</v>
+        <v>0.57697188854217529</v>
       </c>
       <c r="J25">
-        <v>0.5610104203224182</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1" t="s">
-        <v>15</v>
+        <v>0.56101042032241821</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26">
-        <v>0.0326966732723725</v>
+        <v>3.2696673272372502E-2</v>
       </c>
       <c r="E26">
-        <v>0.0325038832380075</v>
+        <v>3.25038832380075E-2</v>
       </c>
       <c r="F26">
-        <v>0.07013502996449129</v>
+        <v>7.0135029964491294E-2</v>
       </c>
       <c r="G26">
-        <v>0.4772884547710418</v>
+        <v>0.47728845477104181</v>
       </c>
       <c r="H26">
-        <v>0.5283836722373962</v>
+        <v>0.52838367223739624</v>
       </c>
       <c r="I26">
-        <v>0.5244178175926208</v>
+        <v>0.52441781759262085</v>
       </c>
       <c r="J26">
         <v>0.4789946973323822</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27">
+        <v>5.2223922341394599E-2</v>
+      </c>
+      <c r="E27">
+        <v>5.2025218031780403E-2</v>
+      </c>
+      <c r="F27">
+        <v>0.10102102150364251</v>
+      </c>
+      <c r="G27">
+        <v>0.55863499641418457</v>
+      </c>
+      <c r="H27">
+        <v>0.61051416397094727</v>
+      </c>
+      <c r="I27">
+        <v>0.60890018939971924</v>
+      </c>
+      <c r="J27">
+        <v>0.55757433176040649</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D27">
-        <v>0.0522239223413946</v>
-      </c>
-      <c r="E27">
-        <v>0.0520252180317804</v>
-      </c>
-      <c r="F27">
-        <v>0.1010210215036425</v>
-      </c>
-      <c r="G27">
-        <v>0.5586349964141846</v>
-      </c>
-      <c r="H27">
-        <v>0.6105141639709473</v>
-      </c>
-      <c r="I27">
-        <v>0.6089001893997192</v>
-      </c>
-      <c r="J27">
-        <v>0.5575743317604065</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D28">
-        <v>0.0283183411294565</v>
+        <v>2.8318341129456501E-2</v>
       </c>
       <c r="E28">
-        <v>0.0287394829865486</v>
+        <v>2.87394829865486E-2</v>
       </c>
       <c r="F28">
-        <v>0.0641065809455718</v>
+        <v>6.4106580945571798E-2</v>
       </c>
       <c r="G28">
         <v>0.4120133221149444</v>
@@ -1255,268 +1276,268 @@
         <v>0.4590192437171936</v>
       </c>
       <c r="I28">
-        <v>0.447766900062561</v>
+        <v>0.44776690006256098</v>
       </c>
       <c r="J28">
-        <v>0.4132740497589111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1" t="s">
-        <v>16</v>
+        <v>0.41327404975891108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D29">
-        <v>0.047674069779539</v>
+        <v>4.7674069779539002E-2</v>
       </c>
       <c r="E29">
-        <v>0.0374296781739811</v>
+        <v>3.7429678173981101E-2</v>
       </c>
       <c r="F29">
-        <v>0.07896203455890589</v>
+        <v>7.8962034558905894E-2</v>
       </c>
       <c r="G29">
         <v>0.5473484992980957</v>
       </c>
       <c r="H29">
-        <v>0.5832431316375732</v>
+        <v>0.58324313163757324</v>
       </c>
       <c r="I29">
         <v>0.5624699592590332</v>
       </c>
       <c r="J29">
-        <v>0.5245009660720825</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
+        <v>0.52450096607208252</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
       <c r="C30" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D30">
-        <v>0.0716172143857824</v>
+        <v>7.1617214385782405E-2</v>
       </c>
       <c r="E30">
-        <v>0.0528393249476281</v>
+        <v>5.2839324947628101E-2</v>
       </c>
       <c r="F30">
         <v>0.1119131738724137</v>
       </c>
       <c r="G30">
-        <v>0.620580792427063</v>
+        <v>0.62058079242706299</v>
       </c>
       <c r="H30">
-        <v>0.6590608358383179</v>
+        <v>0.65906083583831787</v>
       </c>
       <c r="I30">
-        <v>0.6482383608818054</v>
+        <v>0.64823836088180542</v>
       </c>
       <c r="J30">
-        <v>0.5986351370811462</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+        <v>0.59863513708114624</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
       <c r="C31" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D31">
-        <v>0.0412005105075672</v>
+        <v>4.1200510507567199E-2</v>
       </c>
       <c r="E31">
-        <v>0.0317691195627018</v>
+        <v>3.17691195627018E-2</v>
       </c>
       <c r="F31">
-        <v>0.0708372174674506</v>
+        <v>7.08372174674506E-2</v>
       </c>
       <c r="G31">
-        <v>0.4802264273166656</v>
+        <v>0.48022642731666559</v>
       </c>
       <c r="H31">
-        <v>0.512576699256897</v>
+        <v>0.51257669925689697</v>
       </c>
       <c r="I31">
-        <v>0.4624153077602386</v>
+        <v>0.46241530776023859</v>
       </c>
       <c r="J31">
-        <v>0.4576557278633117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1" t="s">
-        <v>17</v>
+        <v>0.45765572786331171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32">
+        <v>6.1975652211806599E-2</v>
+      </c>
+      <c r="E32">
+        <v>5.3227593600226102E-2</v>
+      </c>
+      <c r="F32">
+        <v>9.0855680109414E-2</v>
+      </c>
+      <c r="G32">
+        <v>0.57829594612121582</v>
+      </c>
+      <c r="H32">
+        <v>0.62989860773086548</v>
+      </c>
+      <c r="I32">
+        <v>0.62068837881088257</v>
+      </c>
+      <c r="J32">
+        <v>0.60139429569244385</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D32">
-        <v>0.0619756522118066</v>
-      </c>
-      <c r="E32">
-        <v>0.0532275936002261</v>
-      </c>
-      <c r="F32">
-        <v>0.090855680109414</v>
-      </c>
-      <c r="G32">
-        <v>0.5782959461212158</v>
-      </c>
-      <c r="H32">
-        <v>0.6298986077308655</v>
-      </c>
-      <c r="I32">
-        <v>0.6206883788108826</v>
-      </c>
-      <c r="J32">
-        <v>0.6013942956924438</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="D33">
-        <v>0.0912438360656751</v>
+        <v>9.1243836065675099E-2</v>
       </c>
       <c r="E33">
-        <v>0.07913480189498071</v>
+        <v>7.9134801894980705E-2</v>
       </c>
       <c r="F33">
         <v>0.131786213610327</v>
       </c>
       <c r="G33">
-        <v>0.6518320441246033</v>
+        <v>0.65183204412460327</v>
       </c>
       <c r="H33">
-        <v>0.7023789882659912</v>
+        <v>0.70237898826599121</v>
       </c>
       <c r="I33">
-        <v>0.7011776566505432</v>
+        <v>0.70117765665054321</v>
       </c>
       <c r="J33">
         <v>0.6749303936958313</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
       <c r="C34" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D34">
-        <v>0.0514545113937391</v>
+        <v>5.1454511393739098E-2</v>
       </c>
       <c r="E34">
-        <v>0.044935268581566</v>
+        <v>4.4935268581565997E-2</v>
       </c>
       <c r="F34">
-        <v>0.07818011018051919</v>
+        <v>7.8180110180519194E-2</v>
       </c>
       <c r="G34">
-        <v>0.5134545564651489</v>
+        <v>0.51345455646514893</v>
       </c>
       <c r="H34">
-        <v>0.5622748732566833</v>
+        <v>0.56227487325668335</v>
       </c>
       <c r="I34">
-        <v>0.5196211338043213</v>
+        <v>0.51962113380432129</v>
       </c>
       <c r="J34">
         <v>0.5375981330871582</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1" t="s">
-        <v>18</v>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D35">
-        <v>0.0218148669257035</v>
+        <v>2.1814866925703499E-2</v>
       </c>
       <c r="E35">
-        <v>0.0169159549962691</v>
+        <v>1.6915954996269099E-2</v>
       </c>
       <c r="F35">
-        <v>0.056639750307342</v>
+        <v>5.6639750307342002E-2</v>
       </c>
       <c r="G35">
         <v>0.3873200118541717</v>
       </c>
       <c r="H35">
-        <v>0.4494363069534302</v>
+        <v>0.44943630695343018</v>
       </c>
       <c r="I35">
-        <v>0.4059976935386657</v>
+        <v>0.40599769353866572</v>
       </c>
       <c r="J35">
-        <v>0.3897570371627807</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
+        <v>0.38975703716278071</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
       <c r="C36" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D36">
-        <v>0.0325086309660938</v>
+        <v>3.2508630966093799E-2</v>
       </c>
       <c r="E36">
-        <v>0.0287471042295307</v>
+        <v>2.8747104229530699E-2</v>
       </c>
       <c r="F36">
-        <v>0.07804181602778611</v>
+        <v>7.8041816027786107E-2</v>
       </c>
       <c r="G36">
-        <v>0.4543661773204803</v>
+        <v>0.45436617732048029</v>
       </c>
       <c r="H36">
         <v>0.5226401686668396</v>
       </c>
       <c r="I36">
-        <v>0.4997953772544861</v>
+        <v>0.49979537725448608</v>
       </c>
       <c r="J36">
-        <v>0.4572497010231018</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
+        <v>0.45724970102310181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
       <c r="C37" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D37">
-        <v>0.0203005871076327</v>
+        <v>2.03005871076327E-2</v>
       </c>
       <c r="E37">
-        <v>0.0161759435569603</v>
+        <v>1.6175943556960299E-2</v>
       </c>
       <c r="F37">
-        <v>0.0505979522274439</v>
+        <v>5.0597952227443899E-2</v>
       </c>
       <c r="G37">
         <v>0.3372074663639068</v>
       </c>
       <c r="H37">
-        <v>0.3960790038108825</v>
+        <v>0.39607900381088251</v>
       </c>
       <c r="I37">
-        <v>0.3319822251796722</v>
+        <v>0.33198222517967219</v>
       </c>
       <c r="J37">
-        <v>0.3411926627159118</v>
+        <v>0.34119266271591181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>